<commit_message>
Update July Extended Experiment
</commit_message>
<xml_diff>
--- a/experiments/data/Heart_disese_bagus_data-UPDATE.xlsx
+++ b/experiments/data/Heart_disese_bagus_data-UPDATE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqrmafru\Dropbox\PhD_papers\viz_rec\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqrmafru\Dropbox\PhD_papers\DiVE\experiments\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="1860" windowWidth="25605" windowHeight="14955" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="1005" yWindow="1860" windowWidth="25605" windowHeight="14955" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,10 @@
     <sheet name="cost" sheetId="6" r:id="rId3"/>
     <sheet name="avg" sheetId="2" r:id="rId4"/>
     <sheet name="max oldpeak" sheetId="4" r:id="rId5"/>
+    <sheet name="flight cost" sheetId="7" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1687,19 +1688,24 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Linear Importance</c:v>
+                  <c:v>Linear
+Importance</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Greedy Diversity</c:v>
+                  <c:v>Greedy
+Diversity</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>DiVE-Greedy</c:v>
+                  <c:v>DiVE
+Greedy</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>DiVE-iSwap</c:v>
+                  <c:v>DiVE
+iSwap</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>DiVE-dSwap</c:v>
+                  <c:v>DiVE
+dSwap</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1769,19 +1775,24 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Linear Importance</c:v>
+                  <c:v>Linear
+Importance</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Greedy Diversity</c:v>
+                  <c:v>Greedy
+Diversity</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>DiVE-Greedy</c:v>
+                  <c:v>DiVE
+Greedy</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>DiVE-iSwap</c:v>
+                  <c:v>DiVE
+iSwap</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>DiVE-dSwap</c:v>
+                  <c:v>DiVE
+dSwap</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1796,10 +1807,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5309553146362298E-2</c:v>
+                  <c:v>0.33095531463623001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8439526824974664E-2</c:v>
+                  <c:v>0.38439526824974701</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.147682426824975</c:v>
@@ -3044,6 +3055,465 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]flight_costs!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Query Cost (CQ)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]flight_costs!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Linear
+Importance</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Greedy
+Diversity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DiVE
+Greedy</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DiVE
+iSwap</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DiVE
+dSwap</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DiVE
+Greedy
+Adaptive</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DiVE
+dSwap
+Adaptive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]flight_costs!$B$2:$H$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>12.325840473175026</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.325840473175026</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.325840473175026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.325840473175026</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5572906970976996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0257290697097652</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5CFF-4E5A-95CA-C214C2BE688A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]flight_costs!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Diversity Cost (CD)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]flight_costs!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Linear
+Importance</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Greedy
+Diversity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DiVE
+Greedy</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DiVE
+iSwap</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DiVE
+dSwap</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DiVE
+Greedy
+Adaptive</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DiVE
+dSwap
+Adaptive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]flight_costs!$B$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33095531463623001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38439526824974701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.147682426824975</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1594267994812242</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.35439526824974699</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.19942679948122</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5CFF-4E5A-95CA-C214C2BE688A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="92"/>
+        <c:overlap val="100"/>
+        <c:axId val="468812048"/>
+        <c:axId val="468811392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="468812048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="468811392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="468811392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU" sz="1400" i="1" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Total time execution (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="9.2402383074767849E-3"/>
+              <c:y val="0.26758616711372613"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="468812048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20532889062626039"/>
+          <c:y val="1.6974801226769091E-3"/>
+          <c:w val="0.6276493685623733"/>
+          <c:h val="0.129204041802467"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3324,6 +3794,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6815,6 +7325,511 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -7090,6 +8105,43 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -7101,19 +8153,34 @@
       <sheetData sheetId="0">
         <row r="1">
           <cell r="B1" t="str">
-            <v>Linear Importance</v>
+            <v>Linear
+Importance</v>
           </cell>
           <cell r="C1" t="str">
-            <v>Greedy Diversity</v>
+            <v>Greedy
+Diversity</v>
           </cell>
           <cell r="D1" t="str">
-            <v>DiVE-Greedy</v>
+            <v>DiVE
+Greedy</v>
           </cell>
           <cell r="E1" t="str">
-            <v>DiVE-iSwap</v>
+            <v>DiVE
+iSwap</v>
           </cell>
           <cell r="F1" t="str">
-            <v>DiVE-dSwap</v>
+            <v>DiVE
+dSwap</v>
+          </cell>
+          <cell r="G1" t="str">
+            <v>DiVE
+Greedy
+Adaptive</v>
+          </cell>
+          <cell r="H1" t="str">
+            <v>DiVE
+dSwap
+Adaptive</v>
           </cell>
         </row>
         <row r="2">
@@ -7135,6 +8202,12 @@
           <cell r="F2">
             <v>12.325840473175026</v>
           </cell>
+          <cell r="G2">
+            <v>7.5572906970976996</v>
+          </cell>
+          <cell r="H2">
+            <v>7.0257290697097652</v>
+          </cell>
         </row>
         <row r="3">
           <cell r="A3" t="str">
@@ -7144,16 +8217,22 @@
             <v>0</v>
           </cell>
           <cell r="C3">
-            <v>3.5309553146362298E-2</v>
+            <v>0.33095531463623001</v>
           </cell>
           <cell r="D3">
-            <v>5.8439526824974664E-2</v>
+            <v>0.38439526824974701</v>
           </cell>
           <cell r="E3">
             <v>1.147682426824975</v>
           </cell>
           <cell r="F3">
             <v>1.1594267994812242</v>
+          </cell>
+          <cell r="G3">
+            <v>0.35439526824974699</v>
+          </cell>
+          <cell r="H3">
+            <v>1.19942679948122</v>
           </cell>
         </row>
       </sheetData>
@@ -7962,7 +9041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="C10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
@@ -7973,4 +9052,20 @@
   <pageSetup paperSize="9" scale="96" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new rectifying bound report
</commit_message>
<xml_diff>
--- a/experiments/data/Heart_disese_bagus_data-UPDATE.xlsx
+++ b/experiments/data/Heart_disese_bagus_data-UPDATE.xlsx
@@ -3317,7 +3317,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1700" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -3350,7 +3350,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -3360,7 +3360,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-AU" sz="1400" i="1" baseline="0">
+                  <a:rPr lang="en-AU" sz="2000" i="1" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -3374,8 +3374,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="9.2402383074767849E-3"/>
-              <c:y val="0.26758616711372613"/>
+              <c:x val="9.2402383074767832E-3"/>
+              <c:y val="0.16746406699162608"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3391,7 +3391,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -3420,7 +3420,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -8110,15 +8110,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:colOff>123824</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>514349</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9059,7 +9059,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
CIKM2018 camera ready version 0.1
</commit_message>
<xml_diff>
--- a/experiments/data/Heart_disese_bagus_data-UPDATE.xlsx
+++ b/experiments/data/Heart_disese_bagus_data-UPDATE.xlsx
@@ -472,6 +472,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -830,6 +831,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1188,6 +1190,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3166,7 +3169,7 @@
                   <c:v>12.325840473175026</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.5572906970976996</c:v>
+                  <c:v>8.8572906970976995</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7.0257290697097652</c:v>
@@ -8203,7 +8206,7 @@
             <v>12.325840473175026</v>
           </cell>
           <cell r="G2">
-            <v>7.5572906970976996</v>
+            <v>8.8572906970976995</v>
           </cell>
           <cell r="H2">
             <v>7.0257290697097652</v>
@@ -8236,7 +8239,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -9059,7 +9062,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>